<commit_message>
Added writing to excel sheet
</commit_message>
<xml_diff>
--- a/Current Patients/TeSt1/DataBases/Data/TeSt1_Anthropometrics_Source.xlsx
+++ b/Current Patients/TeSt1/DataBases/Data/TeSt1_Anthropometrics_Source.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USER\Robert\Documents\GitHub\KetoGator\Back End\Current Patients\TeSt1\DataBases\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USER\Robert\Documents\GitHub\KetoGator\Current Patients\TeSt1\DataBases\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C84F32-8944-4BAD-AC48-59DD8F3B5E93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA65800-ED6E-44D4-B4F2-E6B86C87E68E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Anthropometrics" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -93,37 +88,37 @@
     <t>RP-6/24/2020</t>
   </si>
   <si>
+    <t>KK-6/24/2020</t>
+  </si>
+  <si>
     <t>RP-6/25/2020</t>
   </si>
   <si>
+    <t>KK-6/25/2020</t>
+  </si>
+  <si>
     <t>RP-6/26/2020</t>
   </si>
   <si>
+    <t>KK-6/26/2020</t>
+  </si>
+  <si>
+    <t>Back to original SSF</t>
+  </si>
+  <si>
     <t>RP-6/27/2020</t>
   </si>
   <si>
+    <t>KK-6/27/2020</t>
+  </si>
+  <si>
     <t>RP-6/28/2020</t>
   </si>
   <si>
-    <t>KK-6/24/2020</t>
-  </si>
-  <si>
-    <t>KK-6/25/2020</t>
-  </si>
-  <si>
-    <t>KK-6/26/2020</t>
-  </si>
-  <si>
-    <t>KK-6/27/2020</t>
-  </si>
-  <si>
     <t>KK-6/28/2020</t>
   </si>
   <si>
     <t>Back to original CP</t>
-  </si>
-  <si>
-    <t>Back to original SSF</t>
   </si>
 </sst>
 </file>
@@ -453,7 +448,7 @@
   <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -582,7 +577,7 @@
         <v>21</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.75">
@@ -635,10 +630,10 @@
         <v>60.5</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.75">
@@ -691,13 +686,13 @@
         <v>60.8</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="U4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.75">
@@ -750,7 +745,7 @@
         <v>61.2</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="T5" s="2" t="s">
         <v>29</v>
@@ -806,13 +801,13 @@
         <v>60.9</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="U6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started de-identification process, KGID translation for database.
</commit_message>
<xml_diff>
--- a/Current Patients/TeSt1/DataBases/Data/TeSt1_Anthropometrics_Source.xlsx
+++ b/Current Patients/TeSt1/DataBases/Data/TeSt1_Anthropometrics_Source.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\GitHub\KetoGator\Current Patients\TeSt1\DataBases\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Perf Python Project\KetoGator\Current Patients\TeSt1\DataBases\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E656426B-DA1F-4CD3-B57A-82CBEE361473}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A747D55-1F1A-487C-AD59-CA1A4EF4E74B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Anthropometrics" sheetId="1" r:id="rId1"/>
@@ -448,7 +448,7 @@
   <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="L15" sqref="K15:L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,7 +638,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2">
         <v>44008</v>

</xml_diff>

<commit_message>
Added med load graph, modified Canvas, updated getPatientGraphs on spreadsheet access and on qt5, changed how graphs are being retreived
</commit_message>
<xml_diff>
--- a/Current Patients/TeSt1/DataBases/Data/TeSt1_Anthropometrics_Source.xlsx
+++ b/Current Patients/TeSt1/DataBases/Data/TeSt1_Anthropometrics_Source.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Perf Python Project\KetoGator\Current Patients\TeSt1\DataBases\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USER\Robert\Documents\GitHub\KetoGator\Current Patients\TeSt1\DataBases\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A747D55-1F1A-487C-AD59-CA1A4EF4E74B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8C6086-BD59-4854-A878-77BED6FEBF5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Anthropometrics" sheetId="1" r:id="rId1"/>
@@ -445,16 +445,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U6"/>
+  <dimension ref="A1:U7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="K15:L15"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12.42578125" customWidth="1"/>
     <col min="20" max="20" width="12.28515625" customWidth="1"/>
   </cols>
@@ -529,7 +529,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>44006</v>
+        <v>43914</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -585,7 +585,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>44007</v>
+        <v>43946</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -641,10 +641,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>44008</v>
+        <v>43977</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -756,7 +756,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="2">
-        <v>44010</v>
+        <v>44040</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -808,6 +808,20 @@
       </c>
       <c r="U6" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2">
+        <v>44045</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>62.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>